<commit_message>
Update Transfer Fav Neopay and Bank Nobu
</commit_message>
<xml_diff>
--- a/DataExcel/Login_pin.xlsx
+++ b/DataExcel/Login_pin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nobu\main\Android-Automation\DataExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF727BED-3A72-48A4-9CDF-F9B90E454569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52475FDF-A48A-4660-8E72-E1855BBFD710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{203580D6-4BBC-5342-8FAE-BB19812591D1}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>